<commit_message>
Recipe table fully functional
</commit_message>
<xml_diff>
--- a/data/recipe_list.xlsx
+++ b/data/recipe_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HU517FJ\OneDrive - EY\Desktop\t\hulseman-site\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="14_{4E0B86E8-A170-4B13-AC27-2453BEA09385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{612D75E0-8E7E-400B-85E1-B7E1C30D25E8}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="14_{4E0B86E8-A170-4B13-AC27-2453BEA09385}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E5A6E40A-AAE7-45E4-A689-6E9E59734D7E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Chicken Soup</t>
   </si>
@@ -189,10 +189,13 @@
     <t>step_name</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>Crockpot</t>
+  </si>
+  <si>
+    <t>img_source</t>
+  </si>
+  <si>
+    <t>static/example.jpg</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,10 +544,11 @@
     <col min="4" max="5" width="10.26953125" customWidth="1"/>
     <col min="6" max="6" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -567,13 +571,16 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -595,8 +602,11 @@
       <c r="G2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10001</v>
       </c>
@@ -609,17 +619,17 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
       <c r="F3" t="s">
         <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>10002</v>
       </c>
@@ -632,17 +642,17 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" t="s">
         <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>10003</v>
       </c>
@@ -655,17 +665,17 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
       <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>10004</v>
       </c>
@@ -687,8 +697,11 @@
       <c r="G6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>10005</v>
       </c>
@@ -709,6 +722,9 @@
       </c>
       <c r="G7" t="s">
         <v>27</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -717,6 +733,7 @@
     <hyperlink ref="F5:F7" r:id="rId2" display="www.google.com" xr:uid="{FF12B5CE-3823-41CF-849D-B9446869B5A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1356,16 +1373,16 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1344296E-C402-4B05-8BD6-4ECD9E0491F6}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="8b6e2155-aeea-4c2a-a288-67c132589329"/>
     <ds:schemaRef ds:uri="648b8e95-4738-46ce-a500-26cf62829c60"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>